<commit_message>
Login.feature ve Login.java butun scenario'lari ile hatalar duzeltildi
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/ScenarioStatus.xlsx
+++ b/src/test/java/ApachePOI/ScenarioStatus.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Monster\IdeaProjects\CampusUI\src\test\java\ApachePOI\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="12">
   <si>
     <t>Login as a Teacher</t>
   </si>
@@ -35,12 +35,34 @@
   </si>
   <si>
     <t>Login as an Admin</t>
+  </si>
+  <si>
+    <t>Login as a Teacher (Negative-1)</t>
+  </si>
+  <si>
+    <t>Login as a Teacher (Negative-2)</t>
+  </si>
+  <si>
+    <t>Login as a Student (Negative-1)</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>Login as a Student (Negative-2)</t>
+  </si>
+  <si>
+    <t>Login as an Admin (Negative-1)</t>
+  </si>
+  <si>
+    <t>Login as an Admin (Negative-2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -386,13 +408,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="37.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -428,6 +450,204 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Calendar feature updated with teacher-layout load
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/ScenarioStatus.xlsx
+++ b/src/test/java/ApachePOI/ScenarioStatus.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="14">
   <si>
     <t>Login as a Teacher</t>
   </si>
@@ -414,7 +414,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -753,6 +753,160 @@
         <v>2</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Campus US-8 is ready
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/ScenarioStatus.xlsx
+++ b/src/test/java/ApachePOI/ScenarioStatus.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="19">
   <si>
     <t>Login as a Teacher</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>Navigate through burger menu to see students</t>
+  </si>
+  <si>
+    <t>Upload PDF file to the system as attach</t>
+  </si>
+  <si>
+    <t>Student should see PDF file to the system as attach</t>
   </si>
 </sst>
 </file>
@@ -423,7 +429,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1015,6 +1021,50 @@
         <v>2</v>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>17</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Campus US-8, US-16, US-24 is ready
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/ScenarioStatus.xlsx
+++ b/src/test/java/ApachePOI/ScenarioStatus.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="22">
   <si>
     <t>Login as a Teacher</t>
   </si>
@@ -71,6 +71,21 @@
   </si>
   <si>
     <t>Navigate through burger menu to see students</t>
+  </si>
+  <si>
+    <t>Upload PDF file to the system as attach</t>
+  </si>
+  <si>
+    <t>Student should see PDF file to the system as attach</t>
+  </si>
+  <si>
+    <t>Add new live session</t>
+  </si>
+  <si>
+    <t>Student should see the teacher's add a new live session</t>
+  </si>
+  <si>
+    <t>Taking an excel report of grades</t>
   </si>
 </sst>
 </file>
@@ -423,7 +438,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1015,6 +1030,248 @@
         <v>2</v>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>17</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>21</v>
+      </c>
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>21</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>20</v>
+      </c>
+      <c r="B63" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>19</v>
+      </c>
+      <c r="B64" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>17</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>18</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>19</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>20</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>17</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>18</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>19</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>20</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
assignment feature fixed all test passed
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/ScenarioStatus.xlsx
+++ b/src/test/java/ApachePOI/ScenarioStatus.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="23">
   <si>
     <t>Login as a Teacher</t>
   </si>
@@ -441,7 +441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1297,6 +1297,28 @@
         <v>2</v>
       </c>
     </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>22</v>
+      </c>
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>22</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>